<commit_message>
adds sourceOfFishSite to release table, generates data file and updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_release_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_release_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B92EE41-78CB-4E86-841C-759F5EA460A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED6F895-25C7-4045-B55A-599A17CA963C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="1210" windowWidth="20470" windowHeight="11390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Position of the mark that was applied to the mark group. Levels = c("Whole body", "Nose")</t>
+  </si>
+  <si>
+    <t>sourceOfFishSite</t>
+  </si>
+  <si>
+    <t>Site where fish used for release were from. Levels = c("Feather River Fish Hatchery", "NA")</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -783,10 +789,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -821,10 +827,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -857,190 +863,190 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="9">
+      <c r="I10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="9">
         <v>446</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M10" s="9">
         <v>2154</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="6" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="14">
+      <c r="K11" s="2"/>
+      <c r="L11" s="14">
         <v>44593.500127314815</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M11" s="14">
         <v>45779.583460648151</v>
       </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="9">
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="9">
         <v>4</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M12" s="9">
         <v>7</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -1075,10 +1081,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>56</v>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -1113,15 +1119,15 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1150,11 +1156,21 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1682,7 +1698,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="15"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1710,7 +1726,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1738,7 +1754,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="15"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1766,7 +1782,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="16"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1794,7 +1810,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -2746,7 +2762,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
@@ -28673,22 +28689,50 @@
       <c r="Y998" s="1"/>
       <c r="Z998" s="1"/>
     </row>
+    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="2"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="3"/>
+      <c r="G999" s="3"/>
+      <c r="H999" s="3"/>
+      <c r="I999" s="2"/>
+      <c r="J999" s="3"/>
+      <c r="K999" s="2"/>
+      <c r="L999" s="3"/>
+      <c r="M999" s="3"/>
+      <c r="N999" s="1"/>
+      <c r="O999" s="1"/>
+      <c r="P999" s="1"/>
+      <c r="Q999" s="1"/>
+      <c r="R999" s="1"/>
+      <c r="S999" s="1"/>
+      <c r="T999" s="1"/>
+      <c r="U999" s="1"/>
+      <c r="V999" s="1"/>
+      <c r="W999" s="1"/>
+      <c r="X999" s="1"/>
+      <c r="Y999" s="1"/>
+      <c r="Z999" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C1:C43" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C56:C999 C1:C44" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E998" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E999" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F998" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F999" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H998" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H999" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates release data to address sourceoffishsite missing field
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_release_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_release_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED6F895-25C7-4045-B55A-599A17CA963C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAC83FF-462A-46E9-BC74-563A08723427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1210" windowWidth="20470" windowHeight="11390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19230" yWindow="1605" windowWidth="18315" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -169,9 +169,6 @@
     <t>Run of fish marked. Level = "Fall"</t>
   </si>
   <si>
-    <t>Origin or production type of fish marked. Levels = c("Natural", "Hatchery")</t>
-  </si>
-  <si>
     <t>Site where fish were released. Level = "Lower Feather River Release Site"</t>
   </si>
   <si>
@@ -199,10 +196,7 @@
     <t>Position of the mark that was applied to the mark group. Levels = c("Whole body", "Nose")</t>
   </si>
   <si>
-    <t>sourceOfFishSite</t>
-  </si>
-  <si>
-    <t>Site where fish used for release were from. Levels = c("Feather River Fish Hatchery", "NA")</t>
+    <t xml:space="preserve">Origin or production type of fish marked. Levels = c("Natural", "Hatchery"). All hatchery fish are from FRFH, and all natural fish are caught in the Lower Feather River RST. </t>
   </si>
 </sst>
 </file>
@@ -520,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -602,7 +596,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
@@ -678,7 +672,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -754,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -789,10 +783,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -827,7 +821,7 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>48</v>
@@ -863,189 +857,189 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="9">
+        <v>446</v>
+      </c>
+      <c r="M9" s="9">
+        <v>2154</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="14">
+        <v>44593.500127314815</v>
+      </c>
+      <c r="M10" s="14">
+        <v>45779.583460648151</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="9">
+        <v>4</v>
+      </c>
+      <c r="M11" s="9">
+        <v>7</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="9">
-        <v>446</v>
-      </c>
-      <c r="M10" s="9">
-        <v>2154</v>
-      </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="14">
-        <v>44593.500127314815</v>
-      </c>
-      <c r="M11" s="14">
-        <v>45779.583460648151</v>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="9">
-        <v>4</v>
-      </c>
-      <c r="M12" s="9">
-        <v>7</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1081,9 +1075,9 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1119,15 +1113,15 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1156,21 +1150,11 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1698,7 +1682,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1726,7 +1710,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="15"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1754,7 +1738,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="16"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1782,7 +1766,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="15"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1810,7 +1794,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="16"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -2762,7 +2746,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="4"/>
+      <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
@@ -28689,50 +28673,22 @@
       <c r="Y998" s="1"/>
       <c r="Z998" s="1"/>
     </row>
-    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A999" s="1"/>
-      <c r="B999" s="1"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="3"/>
-      <c r="G999" s="3"/>
-      <c r="H999" s="3"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="3"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="3"/>
-      <c r="M999" s="3"/>
-      <c r="N999" s="1"/>
-      <c r="O999" s="1"/>
-      <c r="P999" s="1"/>
-      <c r="Q999" s="1"/>
-      <c r="R999" s="1"/>
-      <c r="S999" s="1"/>
-      <c r="T999" s="1"/>
-      <c r="U999" s="1"/>
-      <c r="V999" s="1"/>
-      <c r="W999" s="1"/>
-      <c r="X999" s="1"/>
-      <c r="Y999" s="1"/>
-      <c r="Z999" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C56:C999 C1:C44" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C1:C43" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E999" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E998" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F999" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F998" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H999" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H998" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28796,7 +28752,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>

</xml_diff>